<commit_message>
minor updates to board legend; added BOM files and board PDF
</commit_message>
<xml_diff>
--- a/FT232H-basic-bom-Digikey.xlsx
+++ b/FT232H-basic-bom-Digikey.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="67200" windowHeight="39320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Digikey order" sheetId="1" r:id="rId1"/>
+    <sheet name="Build BOM" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="FT232H_basic_bom" localSheetId="0">Sheet1!$G$2:$L$16</definedName>
+    <definedName name="FT232H_basic_bom" localSheetId="1">'Build BOM'!$A$1:$H$27</definedName>
+    <definedName name="FT232H_basic_bom" localSheetId="0">'Digikey order'!$G$2:$L$16</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -37,11 +39,25 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="FT232H-basic-bom.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:adam:personal:proj:eeg:boards:FT232H-basic:FT232H-basic-bom.csv" comma="1" semicolon="1">
+      <textFields count="8">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="115">
   <si>
     <t>Part</t>
   </si>
@@ -323,13 +339,76 @@
   </si>
   <si>
     <t>Resettable Fuse</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>PROD_ID</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>NUF2042XV6SOT563</t>
+  </si>
+  <si>
+    <t>SOT563</t>
+  </si>
+  <si>
+    <t>NUF2042XV6 - USB ESD protection, and Full-speed USB termination.</t>
+  </si>
+  <si>
+    <t>DIO-00821</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>DIO-09003</t>
+  </si>
+  <si>
+    <t>RES-07856</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>FT232H Basic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -353,6 +432,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -362,7 +462,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -370,24 +470,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,6 +519,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="FT232H-basic-bom" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="FT232H-basic-bom" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -723,7 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -1201,4 +1327,663 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18">
+      <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="3">
+        <v>603</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="A5:I29">
+    <sortCondition ref="C5:C29"/>
+  </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="62" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected RX and TX LED circuit
</commit_message>
<xml_diff>
--- a/FT232H-basic-bom-Digikey.xlsx
+++ b/FT232H-basic-bom-Digikey.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="30600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey order" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="119">
   <si>
     <t>Part</t>
   </si>
@@ -323,18 +323,12 @@
     <t>Sparkfun</t>
   </si>
   <si>
-    <t>F2112CT-ND </t>
-  </si>
-  <si>
     <t>Littelfuse</t>
   </si>
   <si>
     <t>F1</t>
   </si>
   <si>
-    <t>1206L050YR Littelfuse</t>
-  </si>
-  <si>
     <t>PTC0603</t>
   </si>
   <si>
@@ -408,6 +402,18 @@
   </si>
   <si>
     <t>470-ohm SMT</t>
+  </si>
+  <si>
+    <t>P470GCT-ND</t>
+  </si>
+  <si>
+    <t>R3, R4</t>
+  </si>
+  <si>
+    <t>0603L050YR Littelfuse</t>
+  </si>
+  <si>
+    <t>F4150CT-ND</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -507,14 +513,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -523,11 +535,13 @@
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -867,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -882,41 +896,41 @@
     <col min="11" max="11" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1103,17 +1117,20 @@
       </c>
     </row>
     <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H9">
         <v>470</v>
       </c>
       <c r="I9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J9" t="s">
         <v>45</v>
@@ -1332,25 +1349,25 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
         <v>88</v>
-      </c>
-      <c r="B18" t="s">
-        <v>89</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" t="s">
         <v>90</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>91</v>
-      </c>
-      <c r="J18" t="s">
-        <v>92</v>
-      </c>
-      <c r="K18" t="s">
-        <v>93</v>
       </c>
       <c r="L18" t="s">
         <v>86</v>
@@ -1378,7 +1395,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1393,12 +1410,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1407,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
@@ -1416,10 +1433,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I4" s="3"/>
     </row>
@@ -1451,7 +1468,7 @@
     <row r="6" spans="1:9">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -1476,7 +1493,7 @@
     <row r="7" spans="1:9">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
@@ -1501,7 +1518,7 @@
     <row r="8" spans="1:9">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
@@ -1526,7 +1543,7 @@
     <row r="9" spans="1:9">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
@@ -1551,7 +1568,7 @@
     <row r="10" spans="1:9">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -1651,7 +1668,7 @@
     <row r="14" spans="1:9">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
@@ -1733,7 +1750,7 @@
         <v>54</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>52</v>
@@ -1743,22 +1760,22 @@
     <row r="18" spans="1:9">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" s="3">
+        <v>109</v>
+      </c>
+      <c r="C18" s="5">
         <v>470</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>52</v>
@@ -1768,22 +1785,22 @@
     <row r="19" spans="1:9">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C19" s="3">
+        <v>110</v>
+      </c>
+      <c r="C19" s="5">
         <v>470</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>52</v>
@@ -1818,7 +1835,7 @@
     <row r="21" spans="1:9">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>10</v>
@@ -1900,7 +1917,7 @@
         <v>32</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>29</v>
@@ -1910,7 +1927,7 @@
     <row r="25" spans="1:9">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>29</v>
@@ -1925,7 +1942,7 @@
         <v>32</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>29</v>
@@ -1938,16 +1955,16 @@
         <v>15</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1971,7 +1988,7 @@
         <v>36</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>

</xml_diff>